<commit_message>
Fix up home page
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Code/github.com/knicklabs/oaddrsig2021/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962B3538-CD41-5B4C-8BC7-4ED75BBD4DBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844FF14D-76F8-0C4C-8804-8A6BA9D97B13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17780" yWindow="9240" windowWidth="33600" windowHeight="18720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17780" yWindow="9240" windowWidth="33600" windowHeight="18720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Poster Presentations" sheetId="3" r:id="rId1"/>
@@ -319,9 +319,6 @@
     <t>View the poster submissions from 2021</t>
   </si>
   <si>
-    <t>Research Special Interest Group O.A.D.D. Logo</t>
-  </si>
-  <si>
     <t>Lorem ipsum dolor sit amet consectetur adipisicing elit. Nemo expedita voluptas culpa sapiente alias molestiae.</t>
   </si>
   <si>
@@ -341,6 +338,9 @@
   </si>
   <si>
     <t>msmissy@example.com</t>
+  </si>
+  <si>
+    <t>2021 RSIG Research Day</t>
   </si>
 </sst>
 </file>
@@ -2324,13 +2324,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B98623-7752-FA41-B92F-BADDA6E7A4F1}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="92.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2351,10 +2351,10 @@
         <v>79</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>83</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -2370,13 +2370,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>85</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2388,7 +2388,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7716EC5B-4EED-764B-94DB-B69C01719BFB}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2404,10 +2404,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>87</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -2415,10 +2415,10 @@
         <v>57</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>89</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve look of PDF preview
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Code/github.com/knicklabs/oaddrsig2021/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FD1534-7197-CC4E-98B8-CBEA417308EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868A5518-4C96-504E-B69F-63DFC297080F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Poster Presentations" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="96">
   <si>
     <t>Title</t>
   </si>
@@ -350,6 +350,12 @@
   </si>
   <si>
     <t>Carrier_Perry-Prevalance_of_Anxiety_Symptoms_in_Youth_with_ASD.pdf</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.brocku.ca</t>
   </si>
 </sst>
 </file>
@@ -458,7 +464,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -511,6 +517,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -729,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
@@ -2406,7 +2413,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2467,10 +2474,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7716EC5B-4EED-764B-94DB-B69C01719BFB}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2480,7 +2487,7 @@
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="21" t="s">
         <v>91</v>
       </c>
@@ -2493,8 +2500,11 @@
       <c r="D1" s="21" t="s">
         <v>87</v>
       </c>
+      <c r="E1" s="21" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2506,11 +2516,15 @@
       </c>
       <c r="D2" s="22" t="s">
         <v>89</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{4D70AA94-D9EA-1E4E-BD8D-97E41B982002}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{0FFAA782-0E1C-0A43-BCB5-C5AC91680982}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix bug with email parsing
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Code/github.com/knicklabs/oaddrsig2021/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB13ADB-ACAE-2741-B6CF-FF47E73B37F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A414ACF-EA87-054C-9902-401406A903A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22640" yWindow="2440" windowWidth="33600" windowHeight="18780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Submissions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="243">
   <si>
     <t>RSIG Abstract Submission Tracking 2021</t>
   </si>
@@ -840,6 +840,9 @@
   </si>
   <si>
     <t>Minott_Poster.pdf</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -968,7 +971,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1117,6 +1120,10 @@
     <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16443,8 +16450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AC992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16456,7 +16463,7 @@
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
     <col min="6" max="6" width="60.1640625" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="63" customWidth="1"/>
     <col min="9" max="10" width="9.33203125" customWidth="1"/>
     <col min="11" max="11" width="67.5" customWidth="1"/>
     <col min="12" max="12" width="13.5" customWidth="1"/>
@@ -16468,7 +16475,7 @@
         <v>122</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>4</v>
+        <v>242</v>
       </c>
       <c r="C1" s="32" t="s">
         <v>123</v>
@@ -16483,7 +16490,7 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="62" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -16531,7 +16538,7 @@
       <c r="G2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="44" t="s">
         <v>39</v>
       </c>
       <c r="I2" s="21" t="s">
@@ -16592,7 +16599,7 @@
       <c r="G3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="44" t="s">
         <v>44</v>
       </c>
       <c r="I3" s="21" t="s">
@@ -16655,7 +16662,7 @@
       <c r="G4" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="44" t="s">
         <v>49</v>
       </c>
       <c r="I4" s="21" t="s">
@@ -17084,7 +17091,7 @@
       <c r="G11" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="44" t="s">
         <v>34</v>
       </c>
       <c r="I11" s="21" t="s">

</xml_diff>